<commit_message>
type: feat Batch size=12288 seed = 0 optimiaer = Adam
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18ABDFA-8959-6542-915C-D03F2D84CCC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24061CCA-AB4A-2E4F-A535-9D37FBA1B778}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="4420" windowWidth="28040" windowHeight="17440" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Model</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Overall accuracy</t>
+  </si>
+  <si>
+    <t>batch size</t>
+  </si>
+  <si>
+    <t>Diff.</t>
   </si>
 </sst>
 </file>
@@ -56,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -82,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -105,18 +111,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,101 +451,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430593F-7819-094C-821C-EF73CC7AB90A}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
+        <v>128</v>
+      </c>
+      <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="2">
         <v>0.74</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="2">
         <v>0.66100000000000003</v>
       </c>
+      <c r="F3" s="7">
+        <f>D3-E3</f>
+        <v>7.8999999999999959E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
+        <v>128</v>
+      </c>
+      <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="2">
         <v>0.74</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="2">
         <v>0.66100000000000003</v>
       </c>
+      <c r="F4" s="7">
+        <f t="shared" ref="F4:F7" si="0">D4-E4</f>
+        <v>7.8999999999999959E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
+        <v>128</v>
+      </c>
+      <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="2">
         <v>0.70799999999999996</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="2">
         <v>0.68300000000000005</v>
       </c>
+      <c r="F5" s="7">
+        <f t="shared" si="0"/>
+        <v>2.4999999999999911E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
+        <v>128</v>
+      </c>
+      <c r="C6" s="1">
         <v>1024</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="2">
         <v>0.67600000000000005</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="2">
         <v>0.66500000000000004</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="0"/>
+        <v>1.100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1024</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.9999999999999907E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
type: feat batch size = 1024, Adam, seed=0
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24061CCA-AB4A-2E4F-A535-9D37FBA1B778}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1069BC35-4FAC-A34B-87D8-ED1B4117B872}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Model</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Diff.</t>
+  </si>
+  <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>SGD</t>
   </si>
 </sst>
 </file>
@@ -131,12 +140,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,31 +460,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430593F-7819-094C-821C-EF73CC7AB90A}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,126 +493,192 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>128</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0.74</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>0.66100000000000003</v>
       </c>
-      <c r="F3" s="7">
-        <f>D3-E3</f>
+      <c r="G3" s="6">
+        <f>E3-F3</f>
         <v>7.8999999999999959E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>128</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>0.74</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.66100000000000003</v>
       </c>
-      <c r="F4" s="7">
-        <f t="shared" ref="F4:F7" si="0">D4-E4</f>
+      <c r="G4" s="6">
+        <f t="shared" ref="G4:G7" si="0">E4-F4</f>
         <v>7.8999999999999959E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
         <v>128</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>0.70799999999999996</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>0.68300000000000005</v>
       </c>
-      <c r="F5" s="7">
+      <c r="G5" s="6">
         <f t="shared" si="0"/>
         <v>2.4999999999999911E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
         <v>128</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
         <v>1024</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>0.67600000000000005</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>0.66500000000000004</v>
       </c>
-      <c r="F6" s="7">
+      <c r="G6" s="6">
         <f t="shared" si="0"/>
         <v>1.100000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>1024</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4">
         <v>0</v>
       </c>
-      <c r="D7" s="6">
+      <c r="E7" s="5">
         <v>0.68500000000000005</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F7" s="5">
         <v>0.70499999999999996</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="6">
         <f t="shared" si="0"/>
         <v>-1.9999999999999907E-2</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1024</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" ref="G8:G9" si="1">E8-F8</f>
+        <v>-1.5999999999999903E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4">
+        <v>12244</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="1"/>
+        <v>-9.5000000000000084E-2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
type: feat Batch size = 32, seed=0,optim=Adam
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1069BC35-4FAC-A34B-87D8-ED1B4117B872}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A9C4A2-E3CE-6E44-B7D4-5A26C5A12625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Model</t>
   </si>
@@ -463,7 +463,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -618,14 +618,14 @@
         <v>0</v>
       </c>
       <c r="E7" s="5">
-        <v>0.68500000000000005</v>
+        <v>0.748</v>
       </c>
       <c r="F7" s="5">
-        <v>0.70499999999999996</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
-        <v>-1.9999999999999907E-2</v>
+        <v>5.9000000000000052E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -642,39 +642,24 @@
         <v>0</v>
       </c>
       <c r="E8" s="5">
-        <v>0.67300000000000004</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="F8" s="5">
-        <v>0.68899999999999995</v>
+        <v>0.71399999999999997</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" ref="G8:G9" si="1">E8-F8</f>
-        <v>-1.5999999999999903E-2</v>
+        <v>-3.8999999999999924E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4">
-        <v>12244</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="G9" s="6">
-        <f t="shared" si="1"/>
-        <v>-9.5000000000000084E-2</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
type: feat Print test and valid score
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A9C4A2-E3CE-6E44-B7D4-5A26C5A12625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D86312-BBDF-3B45-BB61-D5E68D58E5FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Model</t>
   </si>
@@ -463,7 +463,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,10 +653,18 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>

</xml_diff>

<commit_message>
type: feat batch size =1024, optim=Adam, seed=0
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D86312-BBDF-3B45-BB61-D5E68D58E5FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430ED7FD-868E-7E4D-8667-30976FD3AD2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Model</t>
   </si>
@@ -463,7 +463,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,18 +653,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4">
-        <v>32</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>

</xml_diff>

<commit_message>
type: feat Batchsize=12288, seed=0,optim=Adam, 20 epochs
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zefuh\workspace\interpretability-of-source-code-transformers\POS Code\Experiments\attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2922BCC3-1C4A-6C4F-8828-0DF6CF41AB10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE731178-4362-4BE0-8FC2-0AA5AF65E6ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20625" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Model</t>
   </si>
@@ -68,6 +62,9 @@
   </si>
   <si>
     <t>Batch size</t>
+  </si>
+  <si>
+    <t>Epochs</t>
   </si>
 </sst>
 </file>
@@ -128,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -143,6 +140,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -468,256 +471,282 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430593F-7819-094C-821C-EF73CC7AB90A}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.375" customWidth="1"/>
+    <col min="5" max="5" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="C1" s="6"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G1" s="8"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>128</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>0.74</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>0.66100000000000003</v>
       </c>
-      <c r="G3" s="3">
-        <f>E3-F3</f>
+      <c r="H3" s="3">
+        <f>F3-G3</f>
         <v>7.8999999999999959E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>128</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>0.74</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>0.66100000000000003</v>
       </c>
-      <c r="G4" s="3">
-        <f t="shared" ref="G4:G8" si="0">E4-F4</f>
+      <c r="H4" s="3">
+        <f t="shared" ref="H4:H8" si="0">F4-G4</f>
         <v>7.8999999999999959E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="4">
         <v>128</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>0.70799999999999996</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>0.68300000000000005</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
         <v>2.4999999999999911E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="4">
         <v>128</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="7">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>1024</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>0.67600000000000005</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>0.66500000000000004</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <f t="shared" si="0"/>
         <v>1.100000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2">
         <v>1024</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="2">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <v>0.67800000000000005</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="5">
         <v>0.67300000000000004</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <f t="shared" si="0"/>
         <v>5.0000000000000044E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2">
         <v>12288</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <v>0.502</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="5">
         <v>0.54300000000000004</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <f t="shared" si="0"/>
         <v>-4.1000000000000036E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2">
         <v>1024</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="2">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <v>0.67500000000000004</v>
       </c>
-      <c r="F9" s="5">
+      <c r="G9" s="5">
         <v>0.71399999999999997</v>
       </c>
-      <c r="G9" s="3">
-        <f t="shared" ref="G9" si="1">E9-F9</f>
+      <c r="H9" s="3">
+        <f t="shared" ref="H9" si="1">F9-G9</f>
         <v>-3.8999999999999924E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A10:G12"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A10:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
type:feat Save the excel report
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zefuh\workspace\interpretability-of-source-code-transformers\POS Code\Experiments\attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE731178-4362-4BE0-8FC2-0AA5AF65E6ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D5DE92-7060-43A3-918F-8EBC0A354032}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20625" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Model</t>
   </si>
@@ -471,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430593F-7819-094C-821C-EF73CC7AB90A}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -574,7 +574,7 @@
         <v>0.66100000000000003</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H8" si="0">F4-G4</f>
+        <f t="shared" ref="H4:H9" si="0">F4-G4</f>
         <v>7.8999999999999959E-2</v>
       </c>
     </row>
@@ -666,7 +666,9 @@
       <c r="B8" s="2">
         <v>12288</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2">
+        <v>10</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
@@ -685,46 +687,63 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2">
-        <v>1024</v>
+        <v>12288</v>
       </c>
       <c r="C9" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
       <c r="F9" s="5">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1024</v>
+      </c>
+      <c r="C10" s="2">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
         <v>0.67500000000000004</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G10" s="5">
         <v>0.71399999999999997</v>
       </c>
-      <c r="H9" s="3">
-        <f t="shared" ref="H9" si="1">F9-G9</f>
+      <c r="H10" s="3">
+        <f t="shared" ref="H10" si="1">F10-G10</f>
         <v>-3.8999999999999924E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -743,10 +762,20 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A10:H12"/>
+    <mergeCell ref="A11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
type: feat Early stop, seed=0, batch size=128, more restrict l1 and l2
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zefuh\workspace\interpretability-of-source-code-transformers\POS Code\Experiments\attachments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39A02DF-71C3-4542-BE07-7C571947F62B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E449BA-0EFA-B74E-A70A-499373D341E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20625" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,12 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -479,22 +485,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430593F-7819-094C-821C-EF73CC7AB90A}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" customWidth="1"/>
-    <col min="3" max="3" width="13.75" customWidth="1"/>
-    <col min="4" max="4" width="10.375" customWidth="1"/>
-    <col min="5" max="5" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="6"/>
@@ -506,7 +512,7 @@
       <c r="G1" s="9"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -559,7 +565,7 @@
         <v>7.8999999999999959E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -586,7 +592,7 @@
         <v>7.8999999999999959E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -613,7 +619,7 @@
         <v>4.599999999999993E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -640,7 +646,7 @@
         <v>2.4999999999999911E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -667,7 +673,7 @@
         <v>1.100000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -694,7 +700,7 @@
         <v>5.0000000000000044E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -721,7 +727,7 @@
         <v>-4.1000000000000036E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
@@ -748,7 +754,7 @@
         <v>1.4000000000000012E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -775,7 +781,7 @@
         <v>-3.8999999999999924E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
@@ -787,7 +793,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -797,7 +803,7 @@
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>

</xml_diff>

<commit_message>
type: feat batchsize=1024,optim=Adam, early stopping
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C70032A-550E-0649-BC0B-E78BFD2E5A80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4DAC11-B1E3-DC43-A221-BAA253678735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
@@ -76,10 +76,13 @@
     <t>Overall accuracy on test</t>
   </si>
   <si>
-    <t>Special setups</t>
-  </si>
-  <si>
     <t>minl2=1e-4,minl1=1e-4</t>
+  </si>
+  <si>
+    <t>Other setups</t>
+  </si>
+  <si>
+    <t>Above + run 5 times each</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -178,6 +181,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430593F-7819-094C-821C-EF73CC7AB90A}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,7 +552,7 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -577,6 +581,7 @@
         <f>F3-G3</f>
         <v>7.8999999999999959E-2</v>
       </c>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -601,7 +606,7 @@
         <v>0.66100000000000003</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H11" si="0">F4-G4</f>
+        <f t="shared" ref="H4:H12" si="0">F4-G4</f>
         <v>7.8999999999999959E-2</v>
       </c>
     </row>
@@ -659,34 +664,37 @@
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4">
+      <c r="A7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9">
         <v>128</v>
       </c>
-      <c r="C7" s="7">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1">
-        <v>1</v>
+      <c r="E7" s="9">
+        <v>0</v>
       </c>
       <c r="F7" s="3">
-        <v>0.70799999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="G7" s="3">
-        <v>0.68300000000000005</v>
+        <v>0.72199999999999998</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="0"/>
-        <v>2.4999999999999911E-2</v>
+        <v>-2.200000000000002E-2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -703,44 +711,44 @@
         <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>1024</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3">
-        <v>0.67600000000000005</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="G8" s="3">
-        <v>0.66500000000000004</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="0"/>
-        <v>1.100000000000001E-2</v>
+        <v>2.4999999999999911E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="4">
+        <v>128</v>
+      </c>
+      <c r="C9" s="7">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1">
         <v>1024</v>
       </c>
-      <c r="C9" s="2">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.67800000000000005</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0.67300000000000004</v>
+      <c r="F9" s="3">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.66500000000000004</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="0"/>
-        <v>5.0000000000000044E-3</v>
+        <v>1.100000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -748,7 +756,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="2">
-        <v>12288</v>
+        <v>1024</v>
       </c>
       <c r="C10" s="2">
         <v>10</v>
@@ -760,25 +768,25 @@
         <v>0</v>
       </c>
       <c r="F10" s="5">
-        <v>0.502</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="G10" s="5">
-        <v>0.54300000000000004</v>
+        <v>0.67300000000000004</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="0"/>
-        <v>-4.1000000000000036E-2</v>
+        <v>5.0000000000000044E-3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="2">
         <v>12288</v>
       </c>
       <c r="C11" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>7</v>
@@ -787,57 +795,74 @@
         <v>0</v>
       </c>
       <c r="F11" s="5">
-        <v>0.66700000000000004</v>
+        <v>0.502</v>
       </c>
       <c r="G11" s="5">
-        <v>0.65300000000000002</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="0"/>
-        <v>1.4000000000000012E-2</v>
+        <v>-4.1000000000000036E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="2">
-        <v>1024</v>
+        <v>12288</v>
       </c>
       <c r="C12" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2">
         <v>0</v>
       </c>
       <c r="F12" s="5">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1024</v>
+      </c>
+      <c r="C13" s="2">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
         <v>0.67500000000000004</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G13" s="5">
         <v>0.71399999999999997</v>
       </c>
-      <c r="H12" s="3">
-        <f t="shared" ref="H12" si="1">F12-G12</f>
+      <c r="H13" s="3">
+        <f t="shared" ref="H13" si="1">F13-G13</f>
         <v>-3.8999999999999924E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -856,10 +881,20 @@
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A13:H15"/>
+    <mergeCell ref="A14:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
type: feat Save the excel file
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4DAC11-B1E3-DC43-A221-BAA253678735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E387E58B-1D0A-3540-BB37-C94EF50ADB57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>Model</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Adam</t>
-  </si>
-  <si>
-    <t>SGD</t>
   </si>
   <si>
     <t>Independent layer 0 and incremental layer 0 will have the same accuracy 
@@ -116,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -139,22 +136,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -169,19 +173,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430593F-7819-094C-821C-EF73CC7AB90A}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,390 +513,317 @@
     <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="1"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
-        <v>15</v>
+      <c r="I2" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>128</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0.74</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>0.66100000000000003</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <f>F3-G3</f>
         <v>7.8999999999999959E-2</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>128</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0.74</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>0.66100000000000003</v>
       </c>
-      <c r="H4" s="3">
-        <f t="shared" ref="H4:H12" si="0">F4-G4</f>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H10" si="0">F4-G4</f>
         <v>7.8999999999999959E-2</v>
       </c>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>128</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <v>0</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>0.73099999999999998</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>0.68500000000000005</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <f t="shared" si="0"/>
         <v>4.599999999999993E-2</v>
       </c>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="4">
         <v>128</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>0.70799999999999996</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>0.68799999999999994</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <f t="shared" si="0"/>
         <v>2.0000000000000018E-2</v>
       </c>
-      <c r="I6" t="s">
-        <v>14</v>
+      <c r="I6" s="10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="4">
         <v>128</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="4">
         <v>0</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>0.7</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>0.72199999999999998</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <f t="shared" si="0"/>
         <v>-2.200000000000002E-2</v>
       </c>
-      <c r="I7" t="s">
-        <v>16</v>
+      <c r="I7" s="10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
+        <v>1024</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.748</v>
+      </c>
+      <c r="H8" s="2">
+        <f>F8-G8</f>
+        <v>-3.8000000000000034E-2</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5">
         <v>128</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C9" s="5">
         <v>10</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="4">
         <v>1</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F9" s="2">
         <v>0.70799999999999996</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G9" s="2">
         <v>0.68300000000000005</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H9" s="2">
         <f t="shared" si="0"/>
         <v>2.4999999999999911E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="5">
         <v>128</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C10" s="5">
         <v>10</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="4">
         <v>1024</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F10" s="2">
         <v>0.67600000000000005</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G10" s="2">
         <v>0.66500000000000004</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H10" s="2">
         <f t="shared" si="0"/>
         <v>1.100000000000001E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1024</v>
-      </c>
-      <c r="C10" s="2">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0.67800000000000005</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0.67300000000000004</v>
-      </c>
-      <c r="H10" s="3">
-        <f t="shared" si="0"/>
-        <v>5.0000000000000044E-3</v>
-      </c>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2">
-        <v>12288</v>
-      </c>
-      <c r="C11" s="2">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0.502</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0.54300000000000004</v>
-      </c>
-      <c r="H11" s="3">
-        <f t="shared" si="0"/>
-        <v>-4.1000000000000036E-2</v>
-      </c>
+      <c r="A11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="2">
-        <v>12288</v>
-      </c>
-      <c r="C12" s="2">
-        <v>20</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0.65300000000000002</v>
-      </c>
-      <c r="H12" s="3">
-        <f t="shared" si="0"/>
-        <v>1.4000000000000012E-2</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1024</v>
-      </c>
-      <c r="C13" s="2">
-        <v>10</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="H13" s="3">
-        <f t="shared" ref="H13" si="1">F13-G13</f>
-        <v>-3.8999999999999924E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A14:H16"/>
+    <mergeCell ref="A11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
type: feat batchsize=16384, early stopping, seed=0,optim=Adam
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EB1D89-397D-264F-AEF6-5D6CC32048F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96A0DC9-E214-D947-840B-966E8812A540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
type: feat batchsize=1024, early stopping, 5 times each, l1l2from0, optim=Adam
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689C7665-9FB3-2647-B611-117591529668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E2924F-8EF0-7B42-94A9-9A463E189DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Above + run 5 times each</t>
+  </si>
+  <si>
+    <t>run 5 times each</t>
   </si>
 </sst>
 </file>
@@ -498,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430593F-7819-094C-821C-EF73CC7AB90A}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,7 +612,7 @@
         <v>0.66100000000000003</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H12" si="0">F4-G4</f>
+        <f t="shared" ref="H4:H13" si="0">F4-G4</f>
         <v>7.8999999999999959E-2</v>
       </c>
       <c r="I4" s="10"/>
@@ -765,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1">
-        <v>16384</v>
+        <v>1024</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
@@ -776,95 +779,108 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="3">
-        <v>0.73899999999999999</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.77400000000000002</v>
-      </c>
-      <c r="H10" s="2">
-        <f>F10-G10</f>
-        <v>-3.5000000000000031E-2</v>
-      </c>
-      <c r="I10" s="10"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="1">
+        <v>16384</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="H11" s="2">
+        <f>F11-G11</f>
+        <v>-3.5000000000000031E-2</v>
+      </c>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5">
         <v>128</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C12" s="5">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="D12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4">
         <v>1</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="2">
         <v>0.70799999999999996</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="2">
         <v>0.68300000000000005</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H12" s="2">
         <f t="shared" si="0"/>
         <v>2.4999999999999911E-2</v>
       </c>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="5">
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="5">
         <v>128</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C13" s="5">
         <v>10</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="D13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4">
         <v>1024</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F13" s="2">
         <v>0.67600000000000005</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G13" s="2">
         <v>0.66500000000000004</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H13" s="2">
         <f t="shared" si="0"/>
         <v>1.100000000000001E-2</v>
       </c>
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -876,10 +892,20 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A13:H15"/>
+    <mergeCell ref="A14:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
type: feat Seed=0,batchsize=128,early topping,l1l2from0,5 times each
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E2924F-8EF0-7B42-94A9-9A463E189DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B650F043-DF32-A64B-AB09-47CC383FD7B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="20620" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
@@ -501,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430593F-7819-094C-821C-EF73CC7AB90A}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,7 +612,7 @@
         <v>0.66100000000000003</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H13" si="0">F4-G4</f>
+        <f t="shared" ref="H4:H14" si="0">F4-G4</f>
         <v>7.8999999999999959E-2</v>
       </c>
       <c r="I4" s="10"/>
@@ -779,9 +779,16 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="2"/>
+      <c r="F10" s="3">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.753</v>
+      </c>
+      <c r="H10" s="2">
+        <f>F10-G10</f>
+        <v>3.6000000000000032E-2</v>
+      </c>
       <c r="I10" s="10" t="s">
         <v>16</v>
       </c>
@@ -791,7 +798,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1">
-        <v>16384</v>
+        <v>1024</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
@@ -800,97 +807,108 @@
         <v>7</v>
       </c>
       <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.73899999999999999</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0.77400000000000002</v>
-      </c>
-      <c r="H11" s="2">
-        <f>F11-G11</f>
-        <v>-3.5000000000000031E-2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2"/>
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="1">
+        <v>16384</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="H12" s="2">
+        <f>F12-G12</f>
+        <v>-3.5000000000000031E-2</v>
+      </c>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="5">
         <v>128</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C13" s="5">
         <v>10</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="D13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4">
         <v>1</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F13" s="2">
         <v>0.70799999999999996</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G13" s="2">
         <v>0.68300000000000005</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H13" s="2">
         <f t="shared" si="0"/>
         <v>2.4999999999999911E-2</v>
       </c>
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="5">
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="5">
         <v>128</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C14" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="D14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="4">
         <v>1024</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F14" s="2">
         <v>0.67600000000000005</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G14" s="2">
         <v>0.66500000000000004</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H14" s="2">
         <f t="shared" si="0"/>
         <v>1.100000000000001E-2</v>
       </c>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
@@ -902,10 +920,20 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A14:H16"/>
+    <mergeCell ref="A15:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
type: feat batchsize=1024,early stopping, stronger penalty,optim=Adam
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zefuh\workspace\interpretability-of-source-code-transformers\POS Code\Experiments\attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5142E3AB-35B5-425D-A44D-CEFC215F420A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24AC8F6-A670-42A4-806E-8C7B37BFB65D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="495" windowWidth="35835" windowHeight="20625" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
   <si>
     <t>Model</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>Diff.</t>
-  </si>
-  <si>
-    <t>Optimizer</t>
-  </si>
-  <si>
-    <t>Adam</t>
   </si>
   <si>
     <t>Independent layer 0 and incremental layer 0 will have the same accuracy 
@@ -67,16 +61,16 @@
     <t>Overall accuracy on test</t>
   </si>
   <si>
-    <t>minl2=1e-4,minl1=1e-4</t>
-  </si>
-  <si>
     <t>Other setups</t>
   </si>
   <si>
-    <t>Above + run 5 times each</t>
-  </si>
-  <si>
     <t>run 5 times each</t>
+  </si>
+  <si>
+    <t>Stronger penalty</t>
+  </si>
+  <si>
+    <t>Stronger penalty + run 5 times each</t>
   </si>
 </sst>
 </file>
@@ -150,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,6 +156,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -495,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430593F-7819-094C-821C-EF73CC7AB90A}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -506,56 +503,51 @@
     <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.375" customWidth="1"/>
     <col min="3" max="3" width="13.625" customWidth="1"/>
-    <col min="4" max="4" width="10.375" customWidth="1"/>
-    <col min="5" max="5" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.125" customWidth="1"/>
+    <col min="4" max="4" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -565,25 +557,22 @@
       <c r="C3" s="4">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.74</v>
       </c>
       <c r="F3" s="2">
-        <v>0.74</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="G3" s="2">
-        <v>0.66100000000000003</v>
-      </c>
-      <c r="H3" s="2">
-        <f>F3-G3</f>
+        <f>E3-F3</f>
         <v>7.8999999999999959E-2</v>
       </c>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -593,25 +582,22 @@
       <c r="C4" s="4">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.74</v>
       </c>
       <c r="F4" s="2">
-        <v>0.74</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="G4" s="2">
-        <v>0.66100000000000003</v>
-      </c>
-      <c r="H4" s="2">
-        <f t="shared" ref="H4:H15" si="0">F4-G4</f>
+        <f t="shared" ref="G4:G15" si="0">E4-F4</f>
         <v>7.8999999999999959E-2</v>
       </c>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -619,27 +605,24 @@
         <v>128</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.73099999999999998</v>
       </c>
       <c r="F5" s="2">
-        <v>0.73099999999999998</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="G5" s="2">
-        <v>0.68500000000000005</v>
-      </c>
-      <c r="H5" s="2">
         <f t="shared" si="0"/>
         <v>4.599999999999993E-2</v>
       </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -647,29 +630,26 @@
         <v>128</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.70799999999999996</v>
       </c>
       <c r="F6" s="2">
-        <v>0.70799999999999996</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="G6" s="2">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="H6" s="2">
         <f t="shared" si="0"/>
         <v>2.0000000000000018E-2</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -677,29 +657,26 @@
         <v>128</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.7</v>
       </c>
       <c r="F7" s="2">
-        <v>0.7</v>
+        <v>0.72199999999999998</v>
       </c>
       <c r="G7" s="2">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="H7" s="2">
         <f t="shared" si="0"/>
         <v>-2.200000000000002E-2</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -707,29 +684,26 @@
         <v>128</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.76900000000000002</v>
       </c>
       <c r="F8" s="2">
-        <v>0.76900000000000002</v>
+        <v>0.746</v>
       </c>
       <c r="G8" s="2">
-        <v>0.746</v>
-      </c>
-      <c r="H8" s="2">
         <f t="shared" si="0"/>
         <v>2.300000000000002E-2</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
@@ -737,27 +711,24 @@
         <v>1024</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.74299999999999999</v>
       </c>
       <c r="F9" s="2">
-        <v>0.74299999999999999</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="G9" s="2">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="H9" s="2">
         <f t="shared" si="0"/>
         <v>-2.9000000000000026E-2</v>
       </c>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
@@ -765,29 +736,26 @@
         <v>1024</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.71</v>
       </c>
       <c r="F10" s="3">
-        <v>0.71</v>
-      </c>
-      <c r="G10" s="3">
         <v>0.748</v>
       </c>
-      <c r="H10" s="2">
-        <f>F10-G10</f>
+      <c r="G10" s="2">
+        <f>E10-F10</f>
         <v>-3.8000000000000034E-2</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="H10" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -795,40 +763,46 @@
         <v>1024</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.78900000000000003</v>
       </c>
       <c r="F11" s="3">
-        <v>0.78900000000000003</v>
-      </c>
-      <c r="G11" s="3">
         <v>0.753</v>
       </c>
-      <c r="H11" s="2">
-        <f>F11-G11</f>
+      <c r="G11" s="2">
+        <f>E11-F11</f>
         <v>3.6000000000000032E-2</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="H11" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1024</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+      <c r="H12" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -836,27 +810,24 @@
         <v>16384</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.73899999999999999</v>
       </c>
       <c r="F13" s="3">
-        <v>0.73899999999999999</v>
-      </c>
-      <c r="G13" s="3">
         <v>0.77400000000000002</v>
       </c>
-      <c r="H13" s="2">
-        <f>F13-G13</f>
+      <c r="G13" s="2">
+        <f>E13-F13</f>
         <v>-3.5000000000000031E-2</v>
       </c>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
@@ -866,25 +837,22 @@
       <c r="C14" s="5">
         <v>10</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="D14" s="4">
         <v>1</v>
       </c>
+      <c r="E14" s="2">
+        <v>0.70799999999999996</v>
+      </c>
       <c r="F14" s="2">
-        <v>0.70799999999999996</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="G14" s="2">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="H14" s="2">
         <f t="shared" si="0"/>
         <v>2.4999999999999911E-2</v>
       </c>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -894,60 +862,54 @@
       <c r="C15" s="5">
         <v>10</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="D15" s="4">
         <v>1024</v>
       </c>
+      <c r="E15" s="2">
+        <v>0.67600000000000005</v>
+      </c>
       <c r="F15" s="2">
-        <v>0.67600000000000005</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="G15" s="2">
-        <v>0.66500000000000004</v>
-      </c>
-      <c r="H15" s="2">
         <f t="shared" si="0"/>
         <v>1.100000000000001E-2</v>
       </c>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A16:H18"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A16:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
type: feat batchsize=16384,early stopping, l1l2from0,optim=Adam
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zefuh\workspace\interpretability-of-source-code-transformers\POS Code\Experiments\attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE59B7DE-1454-4642-9FDF-02EE53A1FE8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAD2381-3612-413E-93A5-4009EAC4AEF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="495" windowWidth="35835" windowHeight="20625" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
   <si>
     <t>Model</t>
   </si>
@@ -64,13 +64,13 @@
     <t>Other setups</t>
   </si>
   <si>
-    <t>run 5 times each</t>
-  </si>
-  <si>
     <t>Stronger penalty</t>
   </si>
   <si>
-    <t>Stronger penalty + run 5 times each</t>
+    <t>BO5</t>
+  </si>
+  <si>
+    <t>Stronger penalty + BO5</t>
   </si>
 </sst>
 </file>
@@ -104,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -140,6 +140,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -161,11 +174,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -176,6 +184,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -492,21 +509,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430593F-7819-094C-821C-EF73CC7AB90A}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" customWidth="1"/>
-    <col min="3" max="3" width="13.625" customWidth="1"/>
-    <col min="4" max="4" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.375" customWidth="1"/>
+    <col min="1" max="1" width="10.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="5.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="10"/>
+    <col min="8" max="8" width="30.375" style="10" customWidth="1"/>
+    <col min="9" max="16384" width="11" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -514,12 +533,12 @@
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="7"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -543,7 +562,7 @@
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -570,7 +589,7 @@
         <f>E3-F3</f>
         <v>7.8999999999999959E-2</v>
       </c>
-      <c r="H3" s="8"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -592,10 +611,10 @@
         <v>0.66100000000000003</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G15" si="0">E4-F4</f>
+        <f t="shared" ref="G4:G16" si="0">E4-F4</f>
         <v>7.8999999999999959E-2</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -620,7 +639,7 @@
         <f t="shared" si="0"/>
         <v>4.599999999999993E-2</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -641,12 +660,12 @@
       <c r="F6" s="2">
         <v>0.68799999999999994</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="12">
         <f t="shared" si="0"/>
         <v>2.0000000000000018E-2</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>13</v>
+      <c r="H6" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -662,18 +681,18 @@
       <c r="D7" s="4">
         <v>0</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>0.76900000000000002</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <v>0.746</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="4">
         <f>E7-F7</f>
         <v>2.300000000000002E-2</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>12</v>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -695,11 +714,11 @@
       <c r="F8" s="2">
         <v>0.72199999999999998</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="12">
         <f t="shared" si="0"/>
         <v>-2.200000000000002E-2</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -722,11 +741,11 @@
       <c r="F9" s="2">
         <v>0.77200000000000002</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="12">
         <f t="shared" si="0"/>
         <v>-2.9000000000000026E-2</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -747,43 +766,43 @@
       <c r="F10" s="3">
         <v>0.748</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="12">
         <f>E10-F10</f>
         <v>-3.8000000000000034E-2</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>13</v>
+      <c r="H10" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="A11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4">
         <v>1024</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
         <v>0.78900000000000003</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <v>0.753</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="4">
         <f>E11-F11</f>
         <v>3.6000000000000032E-2</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>12</v>
+      <c r="H11" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="1">
@@ -795,10 +814,17 @@
       <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="7" t="s">
+      <c r="E12" s="3">
+        <v>0.749</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="G12" s="12">
+        <f>E12-F12</f>
+        <v>3.8000000000000034E-2</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -821,95 +847,115 @@
       <c r="F13" s="3">
         <v>0.77400000000000002</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="12">
         <f>E13-F13</f>
         <v>-3.5000000000000031E-2</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="1">
+        <v>16384</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="5">
         <v>128</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C15" s="5">
         <v>10</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D15" s="4">
         <v>1</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E15" s="2">
         <v>0.70799999999999996</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F15" s="2">
         <v>0.68300000000000005</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G15" s="12">
         <f t="shared" si="0"/>
         <v>2.4999999999999911E-2</v>
       </c>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="5">
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5">
         <v>128</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C16" s="5">
         <v>10</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D16" s="4">
         <v>1024</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E16" s="2">
         <v>0.67600000000000005</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F16" s="2">
         <v>0.66500000000000004</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G16" s="12">
         <f t="shared" si="0"/>
         <v>1.100000000000001E-2</v>
       </c>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A16:G18"/>
+    <mergeCell ref="A17:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
type:feat save the excel file
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/SeedInvestigation.xlsx
+++ b/POS Code/Experiments/attachments/SeedInvestigation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zefuh\workspace\interpretability-of-source-code-transformers\POS Code\Experiments\attachments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F0571B-FF59-4A0B-8313-0BB4F5F8702D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7487AB16-D9CF-4644-BAC7-6A61BE9FC309}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20625" activeTab="2" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" activeTab="2" xr2:uid="{7F4400B1-F019-3742-A02D-88C6BE0D31E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="39">
   <si>
     <t>Model</t>
   </si>
@@ -139,6 +145,12 @@
   </si>
   <si>
     <t>BO15</t>
+  </si>
+  <si>
+    <t>BO15 - BO10</t>
+  </si>
+  <si>
+    <t>BO10-BO5</t>
   </si>
 </sst>
 </file>
@@ -292,7 +304,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,6 +384,27 @@
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -384,15 +417,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -414,13 +438,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -431,15 +455,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -764,34 +779,34 @@
       <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="4" customWidth="1"/>
-    <col min="3" max="4" width="13.625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="4" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11" style="4"/>
-    <col min="10" max="10" width="30.375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="30.33203125" style="4" customWidth="1"/>
     <col min="11" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="27"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -823,11 +838,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="39">
         <v>128</v>
       </c>
       <c r="C3" s="3">
@@ -836,7 +851,7 @@
       <c r="D3" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="34">
         <v>0</v>
       </c>
       <c r="F3" s="1">
@@ -854,14 +869,14 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="36"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="29"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="3">
         <v>10</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="27"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="1">
         <v>0.74</v>
       </c>
@@ -877,14 +892,14 @@
       </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="35" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="29"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="27"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="1">
         <v>0.73099999999999998</v>
       </c>
@@ -900,12 +915,12 @@
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="27"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="29"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="1">
         <v>0.70799999999999996</v>
       </c>
@@ -923,12 +938,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="27"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="29"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="1">
         <v>0.7</v>
       </c>
@@ -946,12 +961,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="27"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="29"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="3">
         <v>0.76900000000000002</v>
       </c>
@@ -962,7 +977,7 @@
         <f>F8-G8</f>
         <v>2.300000000000002E-2</v>
       </c>
-      <c r="I8" s="41">
+      <c r="I8" s="28">
         <f>G10-F9</f>
         <v>4.9000000000000044E-2</v>
       </c>
@@ -970,11 +985,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="32"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="29"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="3">
         <v>1</v>
       </c>
@@ -988,14 +1003,14 @@
         <f t="shared" si="0"/>
         <v>-3.3000000000000029E-2</v>
       </c>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="33"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="29"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="3">
         <v>1024</v>
       </c>
@@ -1009,14 +1024,14 @@
         <f t="shared" si="0"/>
         <v>-3.0000000000000027E-3</v>
       </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="32"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="35" t="s">
+      <c r="I10" s="30"/>
+      <c r="J10" s="29"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="29"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="39" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="3">
@@ -1032,17 +1047,17 @@
         <f t="shared" si="0"/>
         <v>5.0000000000000044E-3</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="34">
         <f>G13-F13</f>
         <v>2.300000000000002E-2</v>
       </c>
-      <c r="J11" s="32"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="J11" s="29"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="29"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="3">
         <v>1</v>
       </c>
@@ -1056,14 +1071,14 @@
         <f t="shared" si="0"/>
         <v>-9.000000000000008E-3</v>
       </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="32"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="37"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="29"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="29"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="3">
         <v>1024</v>
       </c>
@@ -1077,19 +1092,19 @@
         <f t="shared" si="0"/>
         <v>-2.300000000000002E-2</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="33"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="34">
+      <c r="I13" s="34"/>
+      <c r="J13" s="30"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="29"/>
+      <c r="B14" s="38">
         <v>1044</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="34">
         <v>0</v>
       </c>
       <c r="F14" s="2">
@@ -1109,12 +1124,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="27"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="29"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="34"/>
       <c r="F15" s="2">
         <v>0.749</v>
       </c>
@@ -1132,12 +1147,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="27"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="29"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="34"/>
       <c r="F16" s="3">
         <v>0.78900000000000003</v>
       </c>
@@ -1148,7 +1163,7 @@
         <f t="shared" si="1"/>
         <v>3.6000000000000032E-2</v>
       </c>
-      <c r="I16" s="41">
+      <c r="I16" s="28">
         <f>G17-G16</f>
         <v>3.7000000000000033E-2</v>
       </c>
@@ -1156,11 +1171,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="32"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="29"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="3">
         <v>1</v>
       </c>
@@ -1174,14 +1189,14 @@
         <f t="shared" si="1"/>
         <v>-1.6000000000000014E-2</v>
       </c>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="33"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="29"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="3">
         <v>1024</v>
       </c>
@@ -1195,14 +1210,14 @@
         <f t="shared" si="1"/>
         <v>-2.8000000000000025E-2</v>
       </c>
-      <c r="I18" s="33"/>
-      <c r="J18" s="32"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="27" t="s">
+      <c r="I18" s="30"/>
+      <c r="J18" s="29"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="29"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="34" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="3">
@@ -1218,17 +1233,17 @@
         <f t="shared" si="1"/>
         <v>-1.0000000000000009E-2</v>
       </c>
-      <c r="I19" s="41">
+      <c r="I19" s="28">
         <f>G19-F21</f>
         <v>4.0000000000000036E-2</v>
       </c>
-      <c r="J19" s="32"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="27"/>
+      <c r="J19" s="29"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="29"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="3">
         <v>1</v>
       </c>
@@ -1242,14 +1257,14 @@
         <f t="shared" si="1"/>
         <v>-5.0000000000000044E-3</v>
       </c>
-      <c r="I20" s="42"/>
-      <c r="J20" s="32"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="27"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="29"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="29"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="3">
         <v>1024</v>
       </c>
@@ -1263,16 +1278,16 @@
         <f t="shared" si="1"/>
         <v>-1.5000000000000013E-2</v>
       </c>
-      <c r="I21" s="43"/>
-      <c r="J21" s="32"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="38">
+      <c r="I21" s="33"/>
+      <c r="J21" s="29"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="29"/>
+      <c r="B22" s="42">
         <v>16384</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="34" t="s">
+      <c r="C22" s="40"/>
+      <c r="D22" s="38" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="3">
@@ -1288,17 +1303,17 @@
         <f t="shared" si="1"/>
         <v>2.1000000000000019E-2</v>
       </c>
-      <c r="I22" s="41">
+      <c r="I22" s="28">
         <f>G24-F24</f>
         <v>4.4000000000000039E-2</v>
       </c>
-      <c r="J22" s="32"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="34"/>
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="29"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="3">
         <v>1</v>
       </c>
@@ -1312,14 +1327,14 @@
         <f t="shared" si="1"/>
         <v>-1.0000000000000009E-3</v>
       </c>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="34"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="29"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="3">
         <v>1024</v>
       </c>
@@ -1333,14 +1348,14 @@
         <f t="shared" si="1"/>
         <v>-4.4000000000000039E-2</v>
       </c>
-      <c r="I24" s="33"/>
-      <c r="J24" s="32"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="38" t="s">
+      <c r="I24" s="30"/>
+      <c r="J24" s="29"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="29"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="42" t="s">
         <v>17</v>
       </c>
       <c r="E25" s="8">
@@ -1356,17 +1371,17 @@
         <f t="shared" si="1"/>
         <v>5.799999999999994E-2</v>
       </c>
-      <c r="I25" s="41">
+      <c r="I25" s="28">
         <f>G27-G25</f>
         <v>0.18499999999999994</v>
       </c>
-      <c r="J25" s="32"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="39"/>
+      <c r="J25" s="29"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="29"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="43"/>
       <c r="E26" s="8">
         <v>1</v>
       </c>
@@ -1380,14 +1395,14 @@
         <f t="shared" si="1"/>
         <v>-4.0000000000000036E-3</v>
       </c>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="40"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="30"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="44"/>
       <c r="E27" s="8">
         <v>1024</v>
       </c>
@@ -1401,54 +1416,46 @@
         <f t="shared" si="1"/>
         <v>-0.14599999999999991</v>
       </c>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
       <c r="I30" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="J16:J27"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="J8:J13"/>
-    <mergeCell ref="I11:I13"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="A28:H30"/>
     <mergeCell ref="E3:E8"/>
@@ -1464,6 +1471,14 @@
     <mergeCell ref="B22:B27"/>
     <mergeCell ref="C5:C27"/>
     <mergeCell ref="D25:D27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="J16:J27"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="J8:J13"/>
+    <mergeCell ref="I11:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1478,47 +1493,47 @@
       <selection activeCell="C24" sqref="A1:I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.125" customWidth="1"/>
-    <col min="9" max="9" width="19.375" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="27"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>27</v>
       </c>
@@ -1541,8 +1556,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -1567,8 +1582,8 @@
         <v>2.8000000000000025E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
       <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
@@ -1582,11 +1597,11 @@
         <f t="shared" ref="E6:E32" si="0">ABS(C6-D6)</f>
         <v>3.7000000000000033E-2</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="34"/>
       <c r="B7" s="11" t="s">
         <v>22</v>
       </c>
@@ -1600,11 +1615,11 @@
         <f t="shared" si="0"/>
         <v>6.5000000000000058E-2</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
       <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
@@ -1618,11 +1633,11 @@
         <f t="shared" si="0"/>
         <v>5.0000000000000044E-3</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="34"/>
       <c r="B9" s="11" t="s">
         <v>23</v>
       </c>
@@ -1636,11 +1651,11 @@
         <f t="shared" si="0"/>
         <v>3.0000000000000027E-3</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="34"/>
       <c r="B10" s="11" t="s">
         <v>24</v>
       </c>
@@ -1654,11 +1669,11 @@
         <f t="shared" si="0"/>
         <v>4.1000000000000036E-2</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
       <c r="B11" s="11" t="s">
         <v>25</v>
       </c>
@@ -1672,11 +1687,11 @@
         <f t="shared" si="0"/>
         <v>1.3000000000000012E-2</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="34" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1701,8 +1716,8 @@
         <v>1.1285714285714296E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="34"/>
       <c r="B13" s="11" t="s">
         <v>21</v>
       </c>
@@ -1716,11 +1731,11 @@
         <f t="shared" si="0"/>
         <v>3.0000000000000027E-3</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="34"/>
       <c r="B14" s="11" t="s">
         <v>22</v>
       </c>
@@ -1734,11 +1749,11 @@
         <f t="shared" si="0"/>
         <v>1.0000000000000009E-3</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="34"/>
       <c r="B15" s="11" t="s">
         <v>4</v>
       </c>
@@ -1752,11 +1767,11 @@
         <f t="shared" si="0"/>
         <v>1.7000000000000015E-2</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="34"/>
       <c r="B16" s="11" t="s">
         <v>23</v>
       </c>
@@ -1770,11 +1785,11 @@
         <f t="shared" si="0"/>
         <v>7.0000000000000062E-3</v>
       </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="34"/>
       <c r="B17" s="11" t="s">
         <v>24</v>
       </c>
@@ -1788,11 +1803,11 @@
         <f t="shared" si="0"/>
         <v>2.200000000000002E-2</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="34"/>
       <c r="B18" s="11" t="s">
         <v>25</v>
       </c>
@@ -1806,11 +1821,11 @@
         <f t="shared" si="0"/>
         <v>1.4000000000000012E-2</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="s">
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="46" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -1835,8 +1850,8 @@
         <v>1.0571428571428565E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="46"/>
       <c r="B20" s="11" t="s">
         <v>21</v>
       </c>
@@ -1850,11 +1865,11 @@
         <f t="shared" si="0"/>
         <v>2.0000000000000018E-3</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="46"/>
       <c r="B21" s="11" t="s">
         <v>22</v>
       </c>
@@ -1868,11 +1883,11 @@
         <f t="shared" si="0"/>
         <v>4.0000000000000036E-3</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="46"/>
       <c r="B22" s="11" t="s">
         <v>4</v>
       </c>
@@ -1886,11 +1901,11 @@
         <f t="shared" si="0"/>
         <v>3.0000000000000027E-3</v>
       </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="46"/>
       <c r="B23" s="11" t="s">
         <v>23</v>
       </c>
@@ -1904,11 +1919,11 @@
         <f t="shared" si="0"/>
         <v>6.0000000000000053E-3</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="46"/>
       <c r="B24" s="11" t="s">
         <v>24</v>
       </c>
@@ -1922,15 +1937,15 @@
         <f t="shared" si="0"/>
         <v>3.5000000000000031E-2</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="46" t="s">
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="I24" s="46"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
+      <c r="I24" s="50"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="46"/>
       <c r="B25" s="11" t="s">
         <v>25</v>
       </c>
@@ -1944,8 +1959,8 @@
         <f t="shared" si="0"/>
         <v>2.1999999999999909E-2</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
       <c r="H25" s="11" t="s">
         <v>2</v>
       </c>
@@ -1953,8 +1968,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="34" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -1970,11 +1985,11 @@
         <f t="shared" si="0"/>
         <v>5.0000000000000044E-3</v>
       </c>
-      <c r="F26" s="48">
+      <c r="F26" s="45">
         <f>E29</f>
         <v>1.0000000000000009E-2</v>
       </c>
-      <c r="G26" s="48">
+      <c r="G26" s="45">
         <f>AVERAGE(E26:E32)</f>
         <v>3.7142857142857177E-3</v>
       </c>
@@ -1987,8 +2002,8 @@
         <v>6.5999999999999948E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="34"/>
       <c r="B27" s="11" t="s">
         <v>21</v>
       </c>
@@ -2002,8 +2017,8 @@
         <f t="shared" si="0"/>
         <v>1.0000000000000009E-3</v>
       </c>
-      <c r="F27" s="48"/>
-      <c r="G27" s="49"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="46"/>
       <c r="H27" s="1">
         <f t="shared" ref="H27:I27" si="1">C20-C27</f>
         <v>3.9000000000000035E-2</v>
@@ -2013,8 +2028,8 @@
         <v>4.0000000000000036E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="34"/>
       <c r="B28" s="11" t="s">
         <v>22</v>
       </c>
@@ -2028,8 +2043,8 @@
         <f t="shared" si="0"/>
         <v>1.0000000000000009E-3</v>
       </c>
-      <c r="F28" s="48"/>
-      <c r="G28" s="49"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="46"/>
       <c r="H28" s="1">
         <f t="shared" ref="H28:I28" si="2">C21-C28</f>
         <v>1.2000000000000011E-2</v>
@@ -2039,8 +2054,8 @@
         <v>9.000000000000008E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="34"/>
       <c r="B29" s="11" t="s">
         <v>4</v>
       </c>
@@ -2054,8 +2069,8 @@
         <f t="shared" si="0"/>
         <v>1.0000000000000009E-2</v>
       </c>
-      <c r="F29" s="48"/>
-      <c r="G29" s="49"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="46"/>
       <c r="H29" s="1">
         <f t="shared" ref="H29:I29" si="3">C22-C29</f>
         <v>3.3000000000000029E-2</v>
@@ -2065,8 +2080,8 @@
         <v>2.6000000000000023E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="34"/>
       <c r="B30" s="11" t="s">
         <v>23</v>
       </c>
@@ -2080,8 +2095,8 @@
         <f t="shared" si="0"/>
         <v>4.0000000000000036E-3</v>
       </c>
-      <c r="F30" s="48"/>
-      <c r="G30" s="49"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="46"/>
       <c r="H30" s="1">
         <f t="shared" ref="H30:I30" si="4">C23-C30</f>
         <v>2.1000000000000019E-2</v>
@@ -2091,8 +2106,8 @@
         <v>1.9000000000000017E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="34"/>
       <c r="B31" s="11" t="s">
         <v>24</v>
       </c>
@@ -2106,8 +2121,8 @@
         <f t="shared" si="0"/>
         <v>2.0000000000000018E-3</v>
       </c>
-      <c r="F31" s="48"/>
-      <c r="G31" s="49"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="46"/>
       <c r="H31" s="1">
         <f t="shared" ref="H31:I31" si="5">C24-C31</f>
         <v>8.6000000000000076E-2</v>
@@ -2117,8 +2132,8 @@
         <v>5.3000000000000047E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="34"/>
       <c r="B32" s="11" t="s">
         <v>25</v>
       </c>
@@ -2132,8 +2147,8 @@
         <f t="shared" si="0"/>
         <v>3.0000000000000027E-3</v>
       </c>
-      <c r="F32" s="48"/>
-      <c r="G32" s="49"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="46"/>
       <c r="H32" s="1">
         <f t="shared" ref="H32:I32" si="6">C25-C32</f>
         <v>4.7000000000000042E-2</v>
@@ -2145,6 +2160,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="G5:G11"/>
+    <mergeCell ref="G12:G18"/>
+    <mergeCell ref="G19:G25"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="F26:F32"/>
     <mergeCell ref="G26:G32"/>
@@ -2155,11 +2175,6 @@
     <mergeCell ref="F5:F11"/>
     <mergeCell ref="F12:F18"/>
     <mergeCell ref="F19:F25"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="G5:G11"/>
-    <mergeCell ref="G12:G18"/>
-    <mergeCell ref="G19:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2167,51 +2182,51 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1B603D-B298-EF4F-AC8B-F9AE80C9FB58}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.625" customWidth="1"/>
-    <col min="3" max="3" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="27"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>27</v>
       </c>
@@ -2234,8 +2249,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -2260,8 +2275,8 @@
         <v>2.8000000000000025E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
       <c r="B6" s="16" t="s">
         <v>21</v>
       </c>
@@ -2275,11 +2290,11 @@
         <f t="shared" ref="E6:E23" si="0">ABS(C6-D6)</f>
         <v>3.7000000000000033E-2</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="34"/>
       <c r="B7" s="16" t="s">
         <v>22</v>
       </c>
@@ -2293,11 +2308,11 @@
         <f t="shared" si="0"/>
         <v>6.5000000000000058E-2</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
       <c r="B8" s="16" t="s">
         <v>4</v>
       </c>
@@ -2311,11 +2326,11 @@
         <f t="shared" si="0"/>
         <v>5.0000000000000044E-3</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="34"/>
       <c r="B9" s="16" t="s">
         <v>23</v>
       </c>
@@ -2329,11 +2344,11 @@
         <f t="shared" si="0"/>
         <v>3.0000000000000027E-3</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="34"/>
       <c r="B10" s="16" t="s">
         <v>24</v>
       </c>
@@ -2347,11 +2362,11 @@
         <f t="shared" si="0"/>
         <v>4.1000000000000036E-2</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
       <c r="B11" s="16" t="s">
         <v>25</v>
       </c>
@@ -2365,11 +2380,11 @@
         <f t="shared" si="0"/>
         <v>1.3000000000000012E-2</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="34" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="16" t="s">
@@ -2394,8 +2409,8 @@
         <v>1.0571428571428565E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="34"/>
       <c r="B13" s="16" t="s">
         <v>21</v>
       </c>
@@ -2409,11 +2424,11 @@
         <f t="shared" si="0"/>
         <v>2.0000000000000018E-3</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="34"/>
       <c r="B14" s="16" t="s">
         <v>22</v>
       </c>
@@ -2427,11 +2442,11 @@
         <f t="shared" si="0"/>
         <v>4.0000000000000036E-3</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="34"/>
       <c r="B15" s="16" t="s">
         <v>4</v>
       </c>
@@ -2445,11 +2460,11 @@
         <f t="shared" si="0"/>
         <v>3.0000000000000027E-3</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="34"/>
       <c r="B16" s="16" t="s">
         <v>23</v>
       </c>
@@ -2463,11 +2478,11 @@
         <f t="shared" si="0"/>
         <v>6.0000000000000053E-3</v>
       </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="34"/>
       <c r="B17" s="16" t="s">
         <v>24</v>
       </c>
@@ -2481,11 +2496,11 @@
         <f t="shared" si="0"/>
         <v>3.5000000000000031E-2</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="34"/>
       <c r="B18" s="16" t="s">
         <v>25</v>
       </c>
@@ -2499,11 +2514,19 @@
         <f t="shared" si="0"/>
         <v>2.1999999999999909E-2</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" s="34"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="34" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="16" t="s">
@@ -2527,9 +2550,25 @@
         <f>AVERAGE(E19:E25)</f>
         <v>1.8285714285714287E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="H19" s="27">
+        <f>C19-C12</f>
+        <v>5.0000000000000044E-3</v>
+      </c>
+      <c r="I19" s="27">
+        <f>D19-D12</f>
+        <v>-5.3999999999999937E-2</v>
+      </c>
+      <c r="J19" s="27">
+        <f>C12-C5</f>
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="K19" s="27">
+        <f>D12-D5</f>
+        <v>6.899999999999995E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="34"/>
       <c r="B20" s="16" t="s">
         <v>21</v>
       </c>
@@ -2543,11 +2582,27 @@
         <f t="shared" si="0"/>
         <v>7.0000000000000062E-3</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="27">
+        <f t="shared" ref="H20:I20" si="1">C20-C13</f>
+        <v>2.0000000000000018E-3</v>
+      </c>
+      <c r="I20" s="27">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000062E-3</v>
+      </c>
+      <c r="J20" s="27">
+        <f t="shared" ref="J20:K20" si="2">C13-C6</f>
+        <v>1.100000000000001E-2</v>
+      </c>
+      <c r="K20" s="27">
+        <f t="shared" si="2"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="34"/>
       <c r="B21" s="16" t="s">
         <v>22</v>
       </c>
@@ -2561,11 +2616,27 @@
         <f t="shared" si="0"/>
         <v>2.4000000000000021E-2</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="27">
+        <f t="shared" ref="H21:I21" si="3">C21-C14</f>
+        <v>2.4000000000000021E-2</v>
+      </c>
+      <c r="I21" s="27">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="J21" s="27">
+        <f t="shared" ref="J21:K21" si="4">C14-C7</f>
+        <v>-6.0000000000000053E-2</v>
+      </c>
+      <c r="K21" s="27">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="34"/>
       <c r="B22" s="16" t="s">
         <v>4</v>
       </c>
@@ -2579,11 +2650,27 @@
         <f t="shared" si="0"/>
         <v>9.000000000000008E-3</v>
       </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="27">
+        <f t="shared" ref="H22:I22" si="5">C22-C15</f>
+        <v>7.0000000000000062E-3</v>
+      </c>
+      <c r="I22" s="27">
+        <f t="shared" si="5"/>
+        <v>-5.0000000000000044E-3</v>
+      </c>
+      <c r="J22" s="27">
+        <f t="shared" ref="J22:K22" si="6">C15-C8</f>
+        <v>1.2000000000000011E-2</v>
+      </c>
+      <c r="K22" s="27">
+        <f t="shared" si="6"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="34"/>
       <c r="B23" s="16" t="s">
         <v>23</v>
       </c>
@@ -2597,11 +2684,27 @@
         <f t="shared" si="0"/>
         <v>1.2000000000000011E-2</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="27">
+        <f t="shared" ref="H23:I23" si="7">C23-C16</f>
+        <v>1.4000000000000012E-2</v>
+      </c>
+      <c r="I23" s="27">
+        <f t="shared" si="7"/>
+        <v>8.0000000000000071E-3</v>
+      </c>
+      <c r="J23" s="27">
+        <f t="shared" ref="J23:K23" si="8">C16-C9</f>
+        <v>1.5000000000000013E-2</v>
+      </c>
+      <c r="K23" s="27">
+        <f t="shared" si="8"/>
+        <v>6.0000000000000053E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="34"/>
       <c r="B24" s="16" t="s">
         <v>24</v>
       </c>
@@ -2615,11 +2718,27 @@
         <f>ABS(C24-D24)</f>
         <v>7.0000000000000062E-3</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="27">
+        <f t="shared" ref="H24:I24" si="9">C24-C17</f>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="I24" s="27">
+        <f t="shared" si="9"/>
+        <v>4.6000000000000041E-2</v>
+      </c>
+      <c r="J24" s="27">
+        <f t="shared" ref="J24:K24" si="10">C17-C10</f>
+        <v>9.1000000000000081E-2</v>
+      </c>
+      <c r="K24" s="27">
+        <f t="shared" si="10"/>
+        <v>1.5000000000000013E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="34"/>
       <c r="B25" s="16" t="s">
         <v>25</v>
       </c>
@@ -2633,22 +2752,40 @@
         <f>ABS(C25-D25)</f>
         <v>1.2000000000000011E-2</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="27">
+        <f t="shared" ref="H25:I25" si="11">C25-C18</f>
+        <v>-1.0000000000000009E-3</v>
+      </c>
+      <c r="I25" s="27">
+        <f t="shared" si="11"/>
+        <v>-1.0999999999999899E-2</v>
+      </c>
+      <c r="J25" s="27">
+        <f t="shared" ref="J25:K25" si="12">C18-C11</f>
+        <v>3.1000000000000028E-2</v>
+      </c>
+      <c r="K25" s="27">
+        <f t="shared" si="12"/>
+        <v>6.5999999999999948E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="F5:F11"/>
+    <mergeCell ref="G5:G11"/>
     <mergeCell ref="G19:G25"/>
     <mergeCell ref="F19:F25"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="F12:F18"/>
     <mergeCell ref="G12:G18"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="F5:F11"/>
-    <mergeCell ref="G5:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>